<commit_message>
restructure for item system and hero system
</commit_message>
<xml_diff>
--- a/_Out/NFDataCfg/Excel/Language.xlsx
+++ b/_Out/NFDataCfg/Excel/Language.xlsx
@@ -4,13 +4,16 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="21495" windowHeight="10335" activeTab="3"/>
+    <workbookView windowWidth="21495" windowHeight="10335" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Property_comm" sheetId="1" r:id="rId1"/>
     <sheet name="Property_hero" sheetId="5" r:id="rId2"/>
-    <sheet name="Property_item" sheetId="3" r:id="rId3"/>
-    <sheet name="Property_task" sheetId="4" r:id="rId4"/>
+    <sheet name="Property_item_gem" sheetId="6" r:id="rId3"/>
+    <sheet name="Property_item_scroll" sheetId="7" r:id="rId4"/>
+    <sheet name="Property_item_supply" sheetId="8" r:id="rId5"/>
+    <sheet name="Property_item_equipment" sheetId="3" r:id="rId6"/>
+    <sheet name="Property_task" sheetId="4" r:id="rId7"/>
   </sheets>
   <calcPr calcId="144525" concurrentCalc="0"/>
 </workbook>
@@ -460,6 +463,435 @@
     <t>要离是人族最悲情的刺客--神魔大战中，自断一臂假意投靠鬼族，然而再次断臂换来重伤夜王.</t>
   </si>
   <si>
+    <t>Desc_GEM_ATK</t>
+  </si>
+  <si>
+    <t>攻击宝石！</t>
+  </si>
+  <si>
+    <t>Desc_GEM_DEF</t>
+  </si>
+  <si>
+    <t>防御宝石！</t>
+  </si>
+  <si>
+    <t>Desc_GEM_FIRE</t>
+  </si>
+  <si>
+    <t>火属性宝石！</t>
+  </si>
+  <si>
+    <t>Desc_GEM_LIGHT</t>
+  </si>
+  <si>
+    <t>雷属性宝石！</t>
+  </si>
+  <si>
+    <t>Desc_GEM_WIND</t>
+  </si>
+  <si>
+    <t>风属性宝石！</t>
+  </si>
+  <si>
+    <t>Desc_GEM_ICE</t>
+  </si>
+  <si>
+    <t>冰属性宝石！</t>
+  </si>
+  <si>
+    <t>Desc_GEM_POISON</t>
+  </si>
+  <si>
+    <t>毒属性宝石！</t>
+  </si>
+  <si>
+    <t>NameID_GEM_ATK</t>
+  </si>
+  <si>
+    <t>攻击宝石</t>
+  </si>
+  <si>
+    <t>NameID_GEM_DEF</t>
+  </si>
+  <si>
+    <t>防御宝石</t>
+  </si>
+  <si>
+    <t>NameID_GEM_FIRE</t>
+  </si>
+  <si>
+    <t>火属性宝石</t>
+  </si>
+  <si>
+    <t>NameID_GEM_LIGHT</t>
+  </si>
+  <si>
+    <t>雷属性宝石</t>
+  </si>
+  <si>
+    <t>NameID_GEM_WIND</t>
+  </si>
+  <si>
+    <t>风属性宝石</t>
+  </si>
+  <si>
+    <t>NameID_GEM_ICE</t>
+  </si>
+  <si>
+    <t>冰属性宝石</t>
+  </si>
+  <si>
+    <t>NameID_GEM_POISON</t>
+  </si>
+  <si>
+    <t>毒属性宝石</t>
+  </si>
+  <si>
+    <t>NameID_HeroCard_1</t>
+  </si>
+  <si>
+    <t>英雄*卡1</t>
+  </si>
+  <si>
+    <t>NameID_HeroCard_2</t>
+  </si>
+  <si>
+    <t>NameID_HeroCard_3</t>
+  </si>
+  <si>
+    <t>NameID_HeroCard_4</t>
+  </si>
+  <si>
+    <t>NameID_HeroCard_5</t>
+  </si>
+  <si>
+    <t>NameID_HeroCard_6</t>
+  </si>
+  <si>
+    <t>NameID_dragon_cannon_1</t>
+  </si>
+  <si>
+    <t>火龙炮(一级)</t>
+  </si>
+  <si>
+    <t>NameID_dragon_cannon_2</t>
+  </si>
+  <si>
+    <t>火龙炮(二级)</t>
+  </si>
+  <si>
+    <t>NameID_dragon_cannon_3</t>
+  </si>
+  <si>
+    <t>火龙炮(三级)</t>
+  </si>
+  <si>
+    <t>NameID_gold_mine_1</t>
+  </si>
+  <si>
+    <t>金矿(一级)</t>
+  </si>
+  <si>
+    <t>NameID_gold_mine_2</t>
+  </si>
+  <si>
+    <t>金矿(二级)</t>
+  </si>
+  <si>
+    <t>NameID_gold_mine_3</t>
+  </si>
+  <si>
+    <t>金矿(三级)</t>
+  </si>
+  <si>
+    <t>NameID_ballista_tower_1</t>
+  </si>
+  <si>
+    <t>箭塔(一级)</t>
+  </si>
+  <si>
+    <t>NameID_ballista_tower_2</t>
+  </si>
+  <si>
+    <t>箭塔(二级)</t>
+  </si>
+  <si>
+    <t>NameID_ballista_tower_3</t>
+  </si>
+  <si>
+    <t>箭塔(三级)</t>
+  </si>
+  <si>
+    <t>NameID_townhall_1</t>
+  </si>
+  <si>
+    <t>庇护所(一级)</t>
+  </si>
+  <si>
+    <t>NameID_townhall_2</t>
+  </si>
+  <si>
+    <t>庇护所(二级)</t>
+  </si>
+  <si>
+    <t>NameID_townhall_3</t>
+  </si>
+  <si>
+    <t>庇护所(三级)</t>
+  </si>
+  <si>
+    <t>NameID_cannon_small_1</t>
+  </si>
+  <si>
+    <t>传送营地(一级)</t>
+  </si>
+  <si>
+    <t>NameID_cannon_small_2</t>
+  </si>
+  <si>
+    <t>传送营地(二级)</t>
+  </si>
+  <si>
+    <t>NameID_cannon_small_3</t>
+  </si>
+  <si>
+    <t>传送营地(三级)</t>
+  </si>
+  <si>
+    <t>NameID_gold_storage_1</t>
+  </si>
+  <si>
+    <t>储金罐(一级)</t>
+  </si>
+  <si>
+    <t>NameID_gold_storage_2</t>
+  </si>
+  <si>
+    <t>储金罐(二级)</t>
+  </si>
+  <si>
+    <t>NameID_gold_storage_3</t>
+  </si>
+  <si>
+    <t>储金罐(三级)</t>
+  </si>
+  <si>
+    <t>NameID_mana_storage_1</t>
+  </si>
+  <si>
+    <t>圣水瓶(一级)</t>
+  </si>
+  <si>
+    <t>NameID_mana_storage_2</t>
+  </si>
+  <si>
+    <t>圣水瓶(二级)</t>
+  </si>
+  <si>
+    <t>NameID_mana_storage_3</t>
+  </si>
+  <si>
+    <t>圣水瓶(三级)</t>
+  </si>
+  <si>
+    <t>NameID_barrack_1</t>
+  </si>
+  <si>
+    <t>军营(一级)</t>
+  </si>
+  <si>
+    <t>NameID_barrack_2</t>
+  </si>
+  <si>
+    <t>军营(二级)</t>
+  </si>
+  <si>
+    <t>NameID_barrack_3</t>
+  </si>
+  <si>
+    <t>军营(三级)</t>
+  </si>
+  <si>
+    <t>NameID_bomb_1</t>
+  </si>
+  <si>
+    <t>炸弹(一级)</t>
+  </si>
+  <si>
+    <t>NameID_bomb_2</t>
+  </si>
+  <si>
+    <t>炸弹(二级)</t>
+  </si>
+  <si>
+    <t>NameID_bomb_3</t>
+  </si>
+  <si>
+    <t>炸弹(三级)</t>
+  </si>
+  <si>
+    <t>NameID_worker_hut_1</t>
+  </si>
+  <si>
+    <t>铁匠铺(一级)</t>
+  </si>
+  <si>
+    <t>NameID_worker_hut_2</t>
+  </si>
+  <si>
+    <t>铁匠铺(二级)</t>
+  </si>
+  <si>
+    <t>NameID_worker_hut_3</t>
+  </si>
+  <si>
+    <t>铁匠铺(三级)</t>
+  </si>
+  <si>
+    <t>NameID_anti_air_tower_1</t>
+  </si>
+  <si>
+    <t>防空火箭(一级)</t>
+  </si>
+  <si>
+    <t>NameID_anti_air_tower_2</t>
+  </si>
+  <si>
+    <t>防空火箭(二级)</t>
+  </si>
+  <si>
+    <t>NameID_anti_air_tower_3</t>
+  </si>
+  <si>
+    <t>防空火箭(三级)</t>
+  </si>
+  <si>
+    <t>NameID_mana_well_1</t>
+  </si>
+  <si>
+    <t>圣水收集器(一级)</t>
+  </si>
+  <si>
+    <t>NameID_mana_well_2</t>
+  </si>
+  <si>
+    <t>圣水收集器(二级)</t>
+  </si>
+  <si>
+    <t>NameID_mana_well_3</t>
+  </si>
+  <si>
+    <t>圣水收集器(三级)</t>
+  </si>
+  <si>
+    <t>Desc_dragon_cannon_1</t>
+  </si>
+  <si>
+    <t>Desc_dragon_cannon_2</t>
+  </si>
+  <si>
+    <t>Desc_dragon_cannon_3</t>
+  </si>
+  <si>
+    <t>Desc_gold_mine_1</t>
+  </si>
+  <si>
+    <t>Desc_gold_mine_2</t>
+  </si>
+  <si>
+    <t>Desc_gold_mine_3</t>
+  </si>
+  <si>
+    <t>Desc_ballista_tower_1</t>
+  </si>
+  <si>
+    <t>Desc_ballista_tower_2</t>
+  </si>
+  <si>
+    <t>Desc_ballista_tower_3</t>
+  </si>
+  <si>
+    <t>Desc_townhall_1</t>
+  </si>
+  <si>
+    <t>Desc_townhall_2</t>
+  </si>
+  <si>
+    <t>Desc_townhall_3</t>
+  </si>
+  <si>
+    <t>Desc_cannon_small_1</t>
+  </si>
+  <si>
+    <t>Desc_cannon_small_2</t>
+  </si>
+  <si>
+    <t>Desc_cannon_small_3</t>
+  </si>
+  <si>
+    <t>Desc_gold_storage_1</t>
+  </si>
+  <si>
+    <t>Desc_gold_storage_2</t>
+  </si>
+  <si>
+    <t>Desc_gold_storage_3</t>
+  </si>
+  <si>
+    <t>Desc_mana_storage_1</t>
+  </si>
+  <si>
+    <t>Desc_mana_storage_2</t>
+  </si>
+  <si>
+    <t>Desc_mana_storage_3</t>
+  </si>
+  <si>
+    <t>Desc_barrack_1</t>
+  </si>
+  <si>
+    <t>Desc_barrack_2</t>
+  </si>
+  <si>
+    <t>Desc_barrack_3</t>
+  </si>
+  <si>
+    <t>Desc_bomb_1</t>
+  </si>
+  <si>
+    <t>Desc_bomb_2</t>
+  </si>
+  <si>
+    <t>Desc_bomb_3</t>
+  </si>
+  <si>
+    <t>Desc_worker_hut_1</t>
+  </si>
+  <si>
+    <t>Desc_worker_hut_2</t>
+  </si>
+  <si>
+    <t>Desc_worker_hut_3</t>
+  </si>
+  <si>
+    <t>Desc_anti_air_tower_1</t>
+  </si>
+  <si>
+    <t>Desc_anti_air_tower_2</t>
+  </si>
+  <si>
+    <t>Desc_anti_air_tower_3</t>
+  </si>
+  <si>
+    <t>Desc_mana_well_1</t>
+  </si>
+  <si>
+    <t>Desc_mana_well_2</t>
+  </si>
+  <si>
+    <t>Desc_mana_well_3</t>
+  </si>
+  <si>
     <t>Desc_Gold_Item1</t>
   </si>
   <si>
@@ -520,48 +952,6 @@
     <t>战争奖励礼包！</t>
   </si>
   <si>
-    <t>Desc_GEM_ATK</t>
-  </si>
-  <si>
-    <t>攻击宝石！</t>
-  </si>
-  <si>
-    <t>Desc_GEM_DEF</t>
-  </si>
-  <si>
-    <t>防御宝石！</t>
-  </si>
-  <si>
-    <t>Desc_GEM_FIRE</t>
-  </si>
-  <si>
-    <t>火属性宝石！</t>
-  </si>
-  <si>
-    <t>Desc_GEM_LIGHT</t>
-  </si>
-  <si>
-    <t>雷属性宝石！</t>
-  </si>
-  <si>
-    <t>Desc_GEM_WIND</t>
-  </si>
-  <si>
-    <t>风属性宝石！</t>
-  </si>
-  <si>
-    <t>Desc_GEM_ICE</t>
-  </si>
-  <si>
-    <t>冰属性宝石！</t>
-  </si>
-  <si>
-    <t>Desc_GEM_POISON</t>
-  </si>
-  <si>
-    <t>毒属性宝石！</t>
-  </si>
-  <si>
     <t>NameID_Gold_Item1</t>
   </si>
   <si>
@@ -620,393 +1010,6 @@
   </si>
   <si>
     <t>战争礼包</t>
-  </si>
-  <si>
-    <t>NameID_GEM_ATK</t>
-  </si>
-  <si>
-    <t>攻击宝石</t>
-  </si>
-  <si>
-    <t>NameID_GEM_DEF</t>
-  </si>
-  <si>
-    <t>防御宝石</t>
-  </si>
-  <si>
-    <t>NameID_GEM_FIRE</t>
-  </si>
-  <si>
-    <t>火属性宝石</t>
-  </si>
-  <si>
-    <t>NameID_GEM_LIGHT</t>
-  </si>
-  <si>
-    <t>雷属性宝石</t>
-  </si>
-  <si>
-    <t>NameID_GEM_WIND</t>
-  </si>
-  <si>
-    <t>风属性宝石</t>
-  </si>
-  <si>
-    <t>NameID_GEM_ICE</t>
-  </si>
-  <si>
-    <t>冰属性宝石</t>
-  </si>
-  <si>
-    <t>NameID_GEM_POISON</t>
-  </si>
-  <si>
-    <t>毒属性宝石</t>
-  </si>
-  <si>
-    <t>NameID_HeroCard_1</t>
-  </si>
-  <si>
-    <t>英雄*卡1</t>
-  </si>
-  <si>
-    <t>NameID_HeroCard_2</t>
-  </si>
-  <si>
-    <t>NameID_HeroCard_3</t>
-  </si>
-  <si>
-    <t>NameID_HeroCard_4</t>
-  </si>
-  <si>
-    <t>NameID_HeroCard_5</t>
-  </si>
-  <si>
-    <t>NameID_HeroCard_6</t>
-  </si>
-  <si>
-    <t>NameID_dragon_cannon_1</t>
-  </si>
-  <si>
-    <t>火龙炮(一级)</t>
-  </si>
-  <si>
-    <t>NameID_dragon_cannon_2</t>
-  </si>
-  <si>
-    <t>火龙炮(二级)</t>
-  </si>
-  <si>
-    <t>NameID_dragon_cannon_3</t>
-  </si>
-  <si>
-    <t>火龙炮(三级)</t>
-  </si>
-  <si>
-    <t>NameID_gold_mine_1</t>
-  </si>
-  <si>
-    <t>金矿(一级)</t>
-  </si>
-  <si>
-    <t>NameID_gold_mine_2</t>
-  </si>
-  <si>
-    <t>金矿(二级)</t>
-  </si>
-  <si>
-    <t>NameID_gold_mine_3</t>
-  </si>
-  <si>
-    <t>金矿(三级)</t>
-  </si>
-  <si>
-    <t>NameID_ballista_tower_1</t>
-  </si>
-  <si>
-    <t>箭塔(一级)</t>
-  </si>
-  <si>
-    <t>NameID_ballista_tower_2</t>
-  </si>
-  <si>
-    <t>箭塔(二级)</t>
-  </si>
-  <si>
-    <t>NameID_ballista_tower_3</t>
-  </si>
-  <si>
-    <t>箭塔(三级)</t>
-  </si>
-  <si>
-    <t>NameID_townhall_1</t>
-  </si>
-  <si>
-    <t>庇护所(一级)</t>
-  </si>
-  <si>
-    <t>NameID_townhall_2</t>
-  </si>
-  <si>
-    <t>庇护所(二级)</t>
-  </si>
-  <si>
-    <t>NameID_townhall_3</t>
-  </si>
-  <si>
-    <t>庇护所(三级)</t>
-  </si>
-  <si>
-    <t>NameID_cannon_small_1</t>
-  </si>
-  <si>
-    <t>传送营地(一级)</t>
-  </si>
-  <si>
-    <t>NameID_cannon_small_2</t>
-  </si>
-  <si>
-    <t>传送营地(二级)</t>
-  </si>
-  <si>
-    <t>NameID_cannon_small_3</t>
-  </si>
-  <si>
-    <t>传送营地(三级)</t>
-  </si>
-  <si>
-    <t>NameID_gold_storage_1</t>
-  </si>
-  <si>
-    <t>储金罐(一级)</t>
-  </si>
-  <si>
-    <t>NameID_gold_storage_2</t>
-  </si>
-  <si>
-    <t>储金罐(二级)</t>
-  </si>
-  <si>
-    <t>NameID_gold_storage_3</t>
-  </si>
-  <si>
-    <t>储金罐(三级)</t>
-  </si>
-  <si>
-    <t>NameID_mana_storage_1</t>
-  </si>
-  <si>
-    <t>圣水瓶(一级)</t>
-  </si>
-  <si>
-    <t>NameID_mana_storage_2</t>
-  </si>
-  <si>
-    <t>圣水瓶(二级)</t>
-  </si>
-  <si>
-    <t>NameID_mana_storage_3</t>
-  </si>
-  <si>
-    <t>圣水瓶(三级)</t>
-  </si>
-  <si>
-    <t>NameID_barrack_1</t>
-  </si>
-  <si>
-    <t>军营(一级)</t>
-  </si>
-  <si>
-    <t>NameID_barrack_2</t>
-  </si>
-  <si>
-    <t>军营(二级)</t>
-  </si>
-  <si>
-    <t>NameID_barrack_3</t>
-  </si>
-  <si>
-    <t>军营(三级)</t>
-  </si>
-  <si>
-    <t>NameID_bomb_1</t>
-  </si>
-  <si>
-    <t>炸弹(一级)</t>
-  </si>
-  <si>
-    <t>NameID_bomb_2</t>
-  </si>
-  <si>
-    <t>炸弹(二级)</t>
-  </si>
-  <si>
-    <t>NameID_bomb_3</t>
-  </si>
-  <si>
-    <t>炸弹(三级)</t>
-  </si>
-  <si>
-    <t>NameID_worker_hut_1</t>
-  </si>
-  <si>
-    <t>铁匠铺(一级)</t>
-  </si>
-  <si>
-    <t>NameID_worker_hut_2</t>
-  </si>
-  <si>
-    <t>铁匠铺(二级)</t>
-  </si>
-  <si>
-    <t>NameID_worker_hut_3</t>
-  </si>
-  <si>
-    <t>铁匠铺(三级)</t>
-  </si>
-  <si>
-    <t>NameID_anti_air_tower_1</t>
-  </si>
-  <si>
-    <t>防空火箭(一级)</t>
-  </si>
-  <si>
-    <t>NameID_anti_air_tower_2</t>
-  </si>
-  <si>
-    <t>防空火箭(二级)</t>
-  </si>
-  <si>
-    <t>NameID_anti_air_tower_3</t>
-  </si>
-  <si>
-    <t>防空火箭(三级)</t>
-  </si>
-  <si>
-    <t>NameID_mana_well_1</t>
-  </si>
-  <si>
-    <t>圣水收集器(一级)</t>
-  </si>
-  <si>
-    <t>NameID_mana_well_2</t>
-  </si>
-  <si>
-    <t>圣水收集器(二级)</t>
-  </si>
-  <si>
-    <t>NameID_mana_well_3</t>
-  </si>
-  <si>
-    <t>圣水收集器(三级)</t>
-  </si>
-  <si>
-    <t>Desc_dragon_cannon_1</t>
-  </si>
-  <si>
-    <t>Desc_dragon_cannon_2</t>
-  </si>
-  <si>
-    <t>Desc_dragon_cannon_3</t>
-  </si>
-  <si>
-    <t>Desc_gold_mine_1</t>
-  </si>
-  <si>
-    <t>Desc_gold_mine_2</t>
-  </si>
-  <si>
-    <t>Desc_gold_mine_3</t>
-  </si>
-  <si>
-    <t>Desc_ballista_tower_1</t>
-  </si>
-  <si>
-    <t>Desc_ballista_tower_2</t>
-  </si>
-  <si>
-    <t>Desc_ballista_tower_3</t>
-  </si>
-  <si>
-    <t>Desc_townhall_1</t>
-  </si>
-  <si>
-    <t>Desc_townhall_2</t>
-  </si>
-  <si>
-    <t>Desc_townhall_3</t>
-  </si>
-  <si>
-    <t>Desc_cannon_small_1</t>
-  </si>
-  <si>
-    <t>Desc_cannon_small_2</t>
-  </si>
-  <si>
-    <t>Desc_cannon_small_3</t>
-  </si>
-  <si>
-    <t>Desc_gold_storage_1</t>
-  </si>
-  <si>
-    <t>Desc_gold_storage_2</t>
-  </si>
-  <si>
-    <t>Desc_gold_storage_3</t>
-  </si>
-  <si>
-    <t>Desc_mana_storage_1</t>
-  </si>
-  <si>
-    <t>Desc_mana_storage_2</t>
-  </si>
-  <si>
-    <t>Desc_mana_storage_3</t>
-  </si>
-  <si>
-    <t>Desc_barrack_1</t>
-  </si>
-  <si>
-    <t>Desc_barrack_2</t>
-  </si>
-  <si>
-    <t>Desc_barrack_3</t>
-  </si>
-  <si>
-    <t>Desc_bomb_1</t>
-  </si>
-  <si>
-    <t>Desc_bomb_2</t>
-  </si>
-  <si>
-    <t>Desc_bomb_3</t>
-  </si>
-  <si>
-    <t>Desc_worker_hut_1</t>
-  </si>
-  <si>
-    <t>Desc_worker_hut_2</t>
-  </si>
-  <si>
-    <t>Desc_worker_hut_3</t>
-  </si>
-  <si>
-    <t>Desc_anti_air_tower_1</t>
-  </si>
-  <si>
-    <t>Desc_anti_air_tower_2</t>
-  </si>
-  <si>
-    <t>Desc_anti_air_tower_3</t>
-  </si>
-  <si>
-    <t>Desc_mana_well_1</t>
-  </si>
-  <si>
-    <t>Desc_mana_well_2</t>
-  </si>
-  <si>
-    <t>Desc_mana_well_3</t>
   </si>
   <si>
     <t>Desc_Task1</t>
@@ -1062,10 +1065,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -1093,18 +1096,17 @@
       <charset val="134"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1115,24 +1117,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1140,14 +1126,6 @@
     <font>
       <b/>
       <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -1163,7 +1141,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1177,9 +1155,70 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1195,42 +1234,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1295,13 +1298,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1313,7 +1370,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1325,43 +1394,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1379,13 +1418,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1397,79 +1448,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1714,6 +1717,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -1734,15 +1746,6 @@
       <top/>
       <bottom style="medium">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1788,15 +1791,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1811,6 +1805,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -1819,145 +1822,145 @@
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="18" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="25" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="18" borderId="25" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="21" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="16" borderId="24" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="18" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -3517,12 +3520,12 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E122"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="10" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="A11" sqref="A11:E12"/>
+      <selection pane="bottomLeft" activeCell="A25" sqref="$A25:$XFD30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="4"/>
@@ -3695,15 +3698,15 @@
       <c r="D10" s="20"/>
       <c r="E10" s="20"/>
     </row>
-    <row r="11" s="22" customFormat="1" spans="1:5">
-      <c r="A11" s="21" t="s">
+    <row r="11" s="25" customFormat="1" spans="1:5">
+      <c r="A11" s="29" t="s">
         <v>144</v>
       </c>
-      <c r="C11" s="23" t="s">
+      <c r="C11" s="26" t="s">
         <v>145</v>
       </c>
-      <c r="D11" s="24"/>
-      <c r="E11" s="24"/>
+      <c r="D11" s="27"/>
+      <c r="E11" s="27"/>
     </row>
     <row r="12" s="25" customFormat="1" spans="1:5">
       <c r="A12" s="29" t="s">
@@ -3715,11 +3718,11 @@
       <c r="D12" s="27"/>
       <c r="E12" s="27"/>
     </row>
-    <row r="13" s="22" customFormat="1" spans="1:5">
-      <c r="A13" s="21" t="s">
+    <row r="13" s="25" customFormat="1" spans="1:5">
+      <c r="A13" s="29" t="s">
         <v>148</v>
       </c>
-      <c r="C13" s="23" t="s">
+      <c r="C13" s="26" t="s">
         <v>149</v>
       </c>
       <c r="D13" s="27"/>
@@ -3752,8 +3755,8 @@
       <c r="C16" s="26" t="s">
         <v>155</v>
       </c>
-      <c r="D16" s="27"/>
-      <c r="E16" s="27"/>
+      <c r="D16"/>
+      <c r="E16"/>
     </row>
     <row r="17" s="25" customFormat="1" spans="1:5">
       <c r="A17" s="29" t="s">
@@ -3762,986 +3765,78 @@
       <c r="C17" s="26" t="s">
         <v>157</v>
       </c>
-      <c r="D17" s="24"/>
-      <c r="E17" s="24"/>
-    </row>
-    <row r="18" s="25" customFormat="1" spans="1:5">
-      <c r="A18" s="29" t="s">
+      <c r="D17"/>
+      <c r="E17"/>
+    </row>
+    <row r="18" s="28" customFormat="1" spans="1:5">
+      <c r="A18" s="30" t="s">
         <v>158</v>
       </c>
-      <c r="C18" s="26" t="s">
+      <c r="C18" s="31" t="s">
         <v>159</v>
       </c>
-      <c r="D18" s="27"/>
-      <c r="E18" s="27"/>
-    </row>
-    <row r="19" s="25" customFormat="1" spans="1:5">
-      <c r="A19" s="29" t="s">
+      <c r="D18"/>
+      <c r="E18"/>
+    </row>
+    <row r="19" s="28" customFormat="1" spans="1:5">
+      <c r="A19" s="30" t="s">
         <v>160</v>
       </c>
-      <c r="C19" s="26" t="s">
+      <c r="C19" s="31" t="s">
         <v>161</v>
       </c>
-      <c r="D19" s="27"/>
-      <c r="E19" s="27"/>
-    </row>
-    <row r="20" s="25" customFormat="1" spans="1:5">
-      <c r="A20" s="29" t="s">
+      <c r="D19"/>
+      <c r="E19"/>
+    </row>
+    <row r="20" s="28" customFormat="1" spans="1:5">
+      <c r="A20" s="30" t="s">
         <v>162</v>
       </c>
-      <c r="C20" s="26" t="s">
+      <c r="C20" s="31" t="s">
         <v>163</v>
       </c>
-      <c r="D20" s="27"/>
-      <c r="E20" s="27"/>
-    </row>
-    <row r="21" s="25" customFormat="1" spans="1:5">
-      <c r="A21" s="29" t="s">
+      <c r="D20"/>
+      <c r="E20"/>
+    </row>
+    <row r="21" s="28" customFormat="1" spans="1:5">
+      <c r="A21" s="30" t="s">
         <v>164</v>
       </c>
-      <c r="C21" s="26" t="s">
+      <c r="C21" s="31" t="s">
         <v>165</v>
       </c>
-      <c r="D21" s="27"/>
-      <c r="E21" s="27"/>
-    </row>
-    <row r="22" s="25" customFormat="1" spans="1:5">
-      <c r="A22" s="29" t="s">
+      <c r="D21"/>
+      <c r="E21"/>
+    </row>
+    <row r="22" s="28" customFormat="1" spans="1:5">
+      <c r="A22" s="30" t="s">
         <v>166</v>
       </c>
-      <c r="C22" s="26" t="s">
+      <c r="C22" s="31" t="s">
         <v>167</v>
       </c>
-      <c r="D22" s="27"/>
-      <c r="E22" s="27"/>
-    </row>
-    <row r="23" s="25" customFormat="1" spans="1:5">
-      <c r="A23" s="29" t="s">
+      <c r="D22"/>
+      <c r="E22"/>
+    </row>
+    <row r="23" s="28" customFormat="1" spans="1:5">
+      <c r="A23" s="30" t="s">
         <v>168</v>
       </c>
-      <c r="C23" s="26" t="s">
+      <c r="C23" s="31" t="s">
         <v>169</v>
       </c>
-      <c r="D23" s="27"/>
-      <c r="E23" s="27"/>
-    </row>
-    <row r="24" s="25" customFormat="1" spans="1:5">
-      <c r="A24" s="29" t="s">
+      <c r="D23"/>
+      <c r="E23"/>
+    </row>
+    <row r="24" s="28" customFormat="1" spans="1:5">
+      <c r="A24" s="30" t="s">
         <v>170</v>
       </c>
-      <c r="C24" s="26" t="s">
+      <c r="C24" s="31" t="s">
         <v>171</v>
       </c>
-      <c r="D24" s="27"/>
-      <c r="E24" s="27"/>
-    </row>
-    <row r="25" s="25" customFormat="1" spans="1:5">
-      <c r="A25" s="29" t="s">
-        <v>172</v>
-      </c>
-      <c r="C25" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="D25" s="27"/>
-      <c r="E25" s="27"/>
-    </row>
-    <row r="26" s="25" customFormat="1" spans="1:5">
-      <c r="A26" s="29" t="s">
-        <v>174</v>
-      </c>
-      <c r="C26" s="26" t="s">
-        <v>175</v>
-      </c>
-      <c r="D26"/>
-      <c r="E26"/>
-    </row>
-    <row r="27" s="25" customFormat="1" spans="1:5">
-      <c r="A27" s="29" t="s">
-        <v>176</v>
-      </c>
-      <c r="C27" s="26" t="s">
-        <v>177</v>
-      </c>
-      <c r="D27"/>
-      <c r="E27"/>
-    </row>
-    <row r="28" s="28" customFormat="1" spans="1:5">
-      <c r="A28" s="30" t="s">
-        <v>178</v>
-      </c>
-      <c r="C28" s="31" t="s">
-        <v>179</v>
-      </c>
-      <c r="D28"/>
-      <c r="E28"/>
-    </row>
-    <row r="29" s="28" customFormat="1" spans="1:5">
-      <c r="A29" s="30" t="s">
-        <v>180</v>
-      </c>
-      <c r="C29" s="31" t="s">
-        <v>181</v>
-      </c>
-      <c r="D29"/>
-      <c r="E29"/>
-    </row>
-    <row r="30" s="28" customFormat="1" spans="1:5">
-      <c r="A30" s="30" t="s">
-        <v>182</v>
-      </c>
-      <c r="C30" s="31" t="s">
-        <v>183</v>
-      </c>
-      <c r="D30"/>
-      <c r="E30"/>
-    </row>
-    <row r="31" s="28" customFormat="1" spans="1:5">
-      <c r="A31" s="30" t="s">
-        <v>184</v>
-      </c>
-      <c r="C31" s="31" t="s">
-        <v>185</v>
-      </c>
-      <c r="D31"/>
-      <c r="E31"/>
-    </row>
-    <row r="32" s="28" customFormat="1" spans="1:5">
-      <c r="A32" s="30" t="s">
-        <v>186</v>
-      </c>
-      <c r="C32" s="31" t="s">
-        <v>187</v>
-      </c>
-      <c r="D32"/>
-      <c r="E32"/>
-    </row>
-    <row r="33" s="28" customFormat="1" spans="1:5">
-      <c r="A33" s="30" t="s">
-        <v>188</v>
-      </c>
-      <c r="C33" s="31" t="s">
-        <v>189</v>
-      </c>
-      <c r="D33"/>
-      <c r="E33"/>
-    </row>
-    <row r="34" s="28" customFormat="1" spans="1:5">
-      <c r="A34" s="30" t="s">
-        <v>190</v>
-      </c>
-      <c r="C34" s="31" t="s">
-        <v>191</v>
-      </c>
-      <c r="D34"/>
-      <c r="E34"/>
-    </row>
-    <row r="35" s="28" customFormat="1" spans="1:5">
-      <c r="A35" s="30" t="s">
-        <v>192</v>
-      </c>
-      <c r="C35" s="31" t="s">
-        <v>193</v>
-      </c>
-      <c r="D35"/>
-      <c r="E35"/>
-    </row>
-    <row r="36" s="28" customFormat="1" spans="1:5">
-      <c r="A36" s="30" t="s">
-        <v>194</v>
-      </c>
-      <c r="C36" s="31" t="s">
-        <v>195</v>
-      </c>
-      <c r="D36"/>
-      <c r="E36"/>
-    </row>
-    <row r="37" s="28" customFormat="1" spans="1:5">
-      <c r="A37" s="30" t="s">
-        <v>196</v>
-      </c>
-      <c r="C37" s="31" t="s">
-        <v>197</v>
-      </c>
-      <c r="D37"/>
-      <c r="E37"/>
-    </row>
-    <row r="38" s="28" customFormat="1" spans="1:5">
-      <c r="A38" s="30" t="s">
-        <v>198</v>
-      </c>
-      <c r="C38" s="31" t="s">
-        <v>199</v>
-      </c>
-      <c r="D38"/>
-      <c r="E38"/>
-    </row>
-    <row r="39" s="28" customFormat="1" spans="1:5">
-      <c r="A39" s="30" t="s">
-        <v>200</v>
-      </c>
-      <c r="C39" s="31" t="s">
-        <v>201</v>
-      </c>
-      <c r="D39"/>
-      <c r="E39"/>
-    </row>
-    <row r="40" s="28" customFormat="1" spans="1:5">
-      <c r="A40" s="30" t="s">
-        <v>202</v>
-      </c>
-      <c r="C40" s="31" t="s">
-        <v>203</v>
-      </c>
-      <c r="D40"/>
-      <c r="E40"/>
-    </row>
-    <row r="41" s="28" customFormat="1" spans="1:5">
-      <c r="A41" s="30" t="s">
-        <v>204</v>
-      </c>
-      <c r="C41" s="31" t="s">
-        <v>205</v>
-      </c>
-      <c r="D41"/>
-      <c r="E41"/>
-    </row>
-    <row r="42" s="28" customFormat="1" spans="1:5">
-      <c r="A42" s="30" t="s">
-        <v>206</v>
-      </c>
-      <c r="C42" s="31" t="s">
-        <v>207</v>
-      </c>
-      <c r="D42"/>
-      <c r="E42"/>
-    </row>
-    <row r="43" s="28" customFormat="1" spans="1:5">
-      <c r="A43" s="30" t="s">
-        <v>208</v>
-      </c>
-      <c r="C43" s="31" t="s">
-        <v>209</v>
-      </c>
-      <c r="D43"/>
-      <c r="E43"/>
-    </row>
-    <row r="44" s="28" customFormat="1" spans="1:5">
-      <c r="A44" s="30" t="s">
-        <v>210</v>
-      </c>
-      <c r="C44" s="31" t="s">
-        <v>211</v>
-      </c>
-      <c r="D44"/>
-      <c r="E44"/>
-    </row>
-    <row r="45" s="28" customFormat="1" spans="1:5">
-      <c r="A45" s="30" t="s">
-        <v>212</v>
-      </c>
-      <c r="C45" s="31" t="s">
-        <v>213</v>
-      </c>
-      <c r="D45"/>
-      <c r="E45"/>
-    </row>
-    <row r="46" s="28" customFormat="1" spans="1:5">
-      <c r="A46" s="30" t="s">
-        <v>214</v>
-      </c>
-      <c r="C46" s="31" t="s">
-        <v>213</v>
-      </c>
-      <c r="D46"/>
-      <c r="E46"/>
-    </row>
-    <row r="47" s="28" customFormat="1" spans="1:5">
-      <c r="A47" s="30" t="s">
-        <v>215</v>
-      </c>
-      <c r="C47" s="31" t="s">
-        <v>213</v>
-      </c>
-      <c r="D47"/>
-      <c r="E47"/>
-    </row>
-    <row r="48" s="28" customFormat="1" spans="1:5">
-      <c r="A48" s="30" t="s">
-        <v>216</v>
-      </c>
-      <c r="C48" s="31" t="s">
-        <v>213</v>
-      </c>
-      <c r="D48"/>
-      <c r="E48"/>
-    </row>
-    <row r="49" s="28" customFormat="1" spans="1:5">
-      <c r="A49" s="30" t="s">
-        <v>217</v>
-      </c>
-      <c r="C49" s="31" t="s">
-        <v>213</v>
-      </c>
-      <c r="D49" s="8"/>
-      <c r="E49" s="8"/>
-    </row>
-    <row r="50" s="28" customFormat="1" spans="1:5">
-      <c r="A50" s="30" t="s">
-        <v>218</v>
-      </c>
-      <c r="C50" s="31" t="s">
-        <v>213</v>
-      </c>
-      <c r="D50" s="8"/>
-      <c r="E50" s="8"/>
-    </row>
-    <row r="51" spans="1:3">
-      <c r="A51" s="32" t="s">
-        <v>219</v>
-      </c>
-      <c r="B51" s="32"/>
-      <c r="C51" s="32" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3">
-      <c r="A52" s="32" t="s">
-        <v>221</v>
-      </c>
-      <c r="B52" s="32"/>
-      <c r="C52" s="32" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3">
-      <c r="A53" s="32" t="s">
-        <v>223</v>
-      </c>
-      <c r="B53" s="32"/>
-      <c r="C53" s="32" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3">
-      <c r="A54" s="32" t="s">
-        <v>225</v>
-      </c>
-      <c r="B54" s="32"/>
-      <c r="C54" s="32" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3">
-      <c r="A55" s="32" t="s">
-        <v>227</v>
-      </c>
-      <c r="B55" s="32"/>
-      <c r="C55" s="32" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3">
-      <c r="A56" s="32" t="s">
-        <v>229</v>
-      </c>
-      <c r="B56" s="32"/>
-      <c r="C56" s="32" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3">
-      <c r="A57" s="32" t="s">
-        <v>231</v>
-      </c>
-      <c r="B57" s="32"/>
-      <c r="C57" s="32" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3">
-      <c r="A58" s="32" t="s">
-        <v>233</v>
-      </c>
-      <c r="B58" s="32"/>
-      <c r="C58" s="32" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3">
-      <c r="A59" s="32" t="s">
-        <v>235</v>
-      </c>
-      <c r="B59" s="32"/>
-      <c r="C59" s="32" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3">
-      <c r="A60" s="32" t="s">
-        <v>237</v>
-      </c>
-      <c r="B60" s="32"/>
-      <c r="C60" s="32" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3">
-      <c r="A61" s="32" t="s">
-        <v>239</v>
-      </c>
-      <c r="B61" s="32"/>
-      <c r="C61" s="32" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3">
-      <c r="A62" s="32" t="s">
-        <v>241</v>
-      </c>
-      <c r="B62" s="32"/>
-      <c r="C62" s="32" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3">
-      <c r="A63" s="32" t="s">
-        <v>243</v>
-      </c>
-      <c r="B63" s="32"/>
-      <c r="C63" s="32" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3">
-      <c r="A64" s="32" t="s">
-        <v>245</v>
-      </c>
-      <c r="B64" s="32"/>
-      <c r="C64" s="32" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3">
-      <c r="A65" s="32" t="s">
-        <v>247</v>
-      </c>
-      <c r="B65" s="32"/>
-      <c r="C65" s="32" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3">
-      <c r="A66" s="32" t="s">
-        <v>249</v>
-      </c>
-      <c r="B66" s="32"/>
-      <c r="C66" s="32" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3">
-      <c r="A67" s="32" t="s">
-        <v>251</v>
-      </c>
-      <c r="B67" s="32"/>
-      <c r="C67" s="32" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3">
-      <c r="A68" s="32" t="s">
-        <v>253</v>
-      </c>
-      <c r="B68" s="32"/>
-      <c r="C68" s="32" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3">
-      <c r="A69" s="32" t="s">
-        <v>255</v>
-      </c>
-      <c r="B69" s="32"/>
-      <c r="C69" s="32" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3">
-      <c r="A70" s="32" t="s">
-        <v>257</v>
-      </c>
-      <c r="B70" s="32"/>
-      <c r="C70" s="32" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3">
-      <c r="A71" s="32" t="s">
-        <v>259</v>
-      </c>
-      <c r="B71" s="32"/>
-      <c r="C71" s="32" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3">
-      <c r="A72" s="32" t="s">
-        <v>261</v>
-      </c>
-      <c r="B72" s="32"/>
-      <c r="C72" s="32" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3">
-      <c r="A73" s="32" t="s">
-        <v>263</v>
-      </c>
-      <c r="B73" s="32"/>
-      <c r="C73" s="32" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3">
-      <c r="A74" s="32" t="s">
-        <v>265</v>
-      </c>
-      <c r="B74" s="32"/>
-      <c r="C74" s="32" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3">
-      <c r="A75" s="32" t="s">
-        <v>267</v>
-      </c>
-      <c r="B75" s="32"/>
-      <c r="C75" s="32" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3">
-      <c r="A76" s="32" t="s">
-        <v>269</v>
-      </c>
-      <c r="B76" s="32"/>
-      <c r="C76" s="32" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3">
-      <c r="A77" s="32" t="s">
-        <v>271</v>
-      </c>
-      <c r="B77" s="32"/>
-      <c r="C77" s="32" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3">
-      <c r="A78" s="32" t="s">
-        <v>273</v>
-      </c>
-      <c r="B78" s="32"/>
-      <c r="C78" s="32" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3">
-      <c r="A79" s="32" t="s">
-        <v>275</v>
-      </c>
-      <c r="B79" s="32"/>
-      <c r="C79" s="32" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3">
-      <c r="A80" s="32" t="s">
-        <v>277</v>
-      </c>
-      <c r="B80" s="32"/>
-      <c r="C80" s="32" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3">
-      <c r="A81" s="32" t="s">
-        <v>279</v>
-      </c>
-      <c r="B81" s="32"/>
-      <c r="C81" s="32" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3">
-      <c r="A82" s="32" t="s">
-        <v>281</v>
-      </c>
-      <c r="B82" s="32"/>
-      <c r="C82" s="32" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3">
-      <c r="A83" s="32" t="s">
-        <v>283</v>
-      </c>
-      <c r="B83" s="32"/>
-      <c r="C83" s="32" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3">
-      <c r="A84" s="32" t="s">
-        <v>285</v>
-      </c>
-      <c r="B84" s="32"/>
-      <c r="C84" s="32" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3">
-      <c r="A85" s="32" t="s">
-        <v>287</v>
-      </c>
-      <c r="B85" s="32"/>
-      <c r="C85" s="32" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3">
-      <c r="A86" s="32" t="s">
-        <v>289</v>
-      </c>
-      <c r="B86" s="32"/>
-      <c r="C86" s="32" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3">
-      <c r="A87" s="32" t="s">
-        <v>291</v>
-      </c>
-      <c r="B87" s="32"/>
-      <c r="C87" s="32" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3">
-      <c r="A88" s="32" t="s">
-        <v>292</v>
-      </c>
-      <c r="B88" s="32"/>
-      <c r="C88" s="32" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3">
-      <c r="A89" s="32" t="s">
-        <v>293</v>
-      </c>
-      <c r="B89" s="32"/>
-      <c r="C89" s="32" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3">
-      <c r="A90" s="32" t="s">
-        <v>294</v>
-      </c>
-      <c r="B90" s="32"/>
-      <c r="C90" s="32" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3">
-      <c r="A91" s="32" t="s">
-        <v>295</v>
-      </c>
-      <c r="B91" s="32"/>
-      <c r="C91" s="32" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3">
-      <c r="A92" s="32" t="s">
-        <v>296</v>
-      </c>
-      <c r="B92" s="32"/>
-      <c r="C92" s="32" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3">
-      <c r="A93" s="32" t="s">
-        <v>297</v>
-      </c>
-      <c r="B93" s="32"/>
-      <c r="C93" s="32" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3">
-      <c r="A94" s="32" t="s">
-        <v>298</v>
-      </c>
-      <c r="B94" s="32"/>
-      <c r="C94" s="32" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3">
-      <c r="A95" s="32" t="s">
-        <v>299</v>
-      </c>
-      <c r="B95" s="32"/>
-      <c r="C95" s="32" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3">
-      <c r="A96" s="32" t="s">
-        <v>300</v>
-      </c>
-      <c r="B96" s="32"/>
-      <c r="C96" s="32" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3">
-      <c r="A97" s="32" t="s">
-        <v>301</v>
-      </c>
-      <c r="B97" s="32"/>
-      <c r="C97" s="32" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3">
-      <c r="A98" s="32" t="s">
-        <v>302</v>
-      </c>
-      <c r="B98" s="32"/>
-      <c r="C98" s="32" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3">
-      <c r="A99" s="32" t="s">
-        <v>303</v>
-      </c>
-      <c r="B99" s="32"/>
-      <c r="C99" s="32" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3">
-      <c r="A100" s="32" t="s">
-        <v>304</v>
-      </c>
-      <c r="B100" s="32"/>
-      <c r="C100" s="32" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3">
-      <c r="A101" s="32" t="s">
-        <v>305</v>
-      </c>
-      <c r="B101" s="32"/>
-      <c r="C101" s="32" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3">
-      <c r="A102" s="32" t="s">
-        <v>306</v>
-      </c>
-      <c r="B102" s="32"/>
-      <c r="C102" s="32" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3">
-      <c r="A103" s="32" t="s">
-        <v>307</v>
-      </c>
-      <c r="B103" s="32"/>
-      <c r="C103" s="32" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3">
-      <c r="A104" s="32" t="s">
-        <v>308</v>
-      </c>
-      <c r="B104" s="32"/>
-      <c r="C104" s="32" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="105" spans="1:3">
-      <c r="A105" s="32" t="s">
-        <v>309</v>
-      </c>
-      <c r="B105" s="32"/>
-      <c r="C105" s="32" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="106" spans="1:3">
-      <c r="A106" s="32" t="s">
-        <v>310</v>
-      </c>
-      <c r="B106" s="32"/>
-      <c r="C106" s="32" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3">
-      <c r="A107" s="32" t="s">
-        <v>311</v>
-      </c>
-      <c r="B107" s="32"/>
-      <c r="C107" s="32" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="108" spans="1:3">
-      <c r="A108" s="32" t="s">
-        <v>312</v>
-      </c>
-      <c r="B108" s="32"/>
-      <c r="C108" s="32" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="109" spans="1:3">
-      <c r="A109" s="32" t="s">
-        <v>313</v>
-      </c>
-      <c r="B109" s="32"/>
-      <c r="C109" s="32" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="110" spans="1:3">
-      <c r="A110" s="32" t="s">
-        <v>314</v>
-      </c>
-      <c r="B110" s="32"/>
-      <c r="C110" s="32" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="111" spans="1:3">
-      <c r="A111" s="32" t="s">
-        <v>315</v>
-      </c>
-      <c r="B111" s="32"/>
-      <c r="C111" s="32" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="112" spans="1:3">
-      <c r="A112" s="32" t="s">
-        <v>316</v>
-      </c>
-      <c r="B112" s="32"/>
-      <c r="C112" s="32" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="113" spans="1:3">
-      <c r="A113" s="32" t="s">
-        <v>317</v>
-      </c>
-      <c r="B113" s="32"/>
-      <c r="C113" s="32" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="114" spans="1:3">
-      <c r="A114" s="32" t="s">
-        <v>318</v>
-      </c>
-      <c r="B114" s="32"/>
-      <c r="C114" s="32" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="115" spans="1:3">
-      <c r="A115" s="32" t="s">
-        <v>319</v>
-      </c>
-      <c r="B115" s="32"/>
-      <c r="C115" s="32" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="116" spans="1:3">
-      <c r="A116" s="32" t="s">
-        <v>320</v>
-      </c>
-      <c r="B116" s="32"/>
-      <c r="C116" s="32" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="117" spans="1:3">
-      <c r="A117" s="32" t="s">
-        <v>321</v>
-      </c>
-      <c r="B117" s="32"/>
-      <c r="C117" s="32" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="118" spans="1:3">
-      <c r="A118" s="32" t="s">
-        <v>322</v>
-      </c>
-      <c r="B118" s="32"/>
-      <c r="C118" s="32" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="119" spans="1:3">
-      <c r="A119" s="32" t="s">
-        <v>323</v>
-      </c>
-      <c r="B119" s="32"/>
-      <c r="C119" s="32" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="120" spans="1:3">
-      <c r="A120" s="32" t="s">
-        <v>324</v>
-      </c>
-      <c r="B120" s="32"/>
-      <c r="C120" s="32" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="121" spans="1:3">
-      <c r="A121" s="32" t="s">
-        <v>325</v>
-      </c>
-      <c r="B121" s="32"/>
-      <c r="C121" s="32" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="122" spans="1:3">
-      <c r="A122" s="32" t="s">
-        <v>326</v>
-      </c>
-      <c r="B122" s="32"/>
-      <c r="C122" s="32" t="s">
-        <v>290</v>
-      </c>
+      <c r="D24"/>
+      <c r="E24"/>
     </row>
   </sheetData>
   <dataValidations count="2">
@@ -4759,9 +3854,1499 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
+  <dimension ref="A1:E88"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="10" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection/>
+      <selection pane="bottomLeft" activeCell="B21" sqref="B21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="4"/>
+  <cols>
+    <col min="1" max="1" width="31.8" style="5" customWidth="1"/>
+    <col min="2" max="2" width="33.3333333333333" style="6" customWidth="1"/>
+    <col min="3" max="3" width="87.4" style="7" customWidth="1"/>
+    <col min="4" max="16384" width="9" style="8"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" spans="1:5">
+      <c r="A1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" s="2" customFormat="1" spans="1:5">
+      <c r="A2" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" s="2" customFormat="1" spans="1:5">
+      <c r="A3" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="2">
+        <v>0</v>
+      </c>
+      <c r="C3" s="15">
+        <v>0</v>
+      </c>
+      <c r="D3" s="15">
+        <v>0</v>
+      </c>
+      <c r="E3" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" s="2" customFormat="1" spans="1:5">
+      <c r="A4" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0</v>
+      </c>
+      <c r="C4" s="15">
+        <v>0</v>
+      </c>
+      <c r="D4" s="15">
+        <v>0</v>
+      </c>
+      <c r="E4" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" s="2" customFormat="1" spans="1:5">
+      <c r="A5" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="2">
+        <v>0</v>
+      </c>
+      <c r="C5" s="15">
+        <v>0</v>
+      </c>
+      <c r="D5" s="15">
+        <v>0</v>
+      </c>
+      <c r="E5" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" s="2" customFormat="1" spans="1:5">
+      <c r="A6" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="2">
+        <v>0</v>
+      </c>
+      <c r="C6" s="15">
+        <v>0</v>
+      </c>
+      <c r="D6" s="15">
+        <v>0</v>
+      </c>
+      <c r="E6" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" s="3" customFormat="1" spans="1:5">
+      <c r="A7" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="3">
+        <v>0</v>
+      </c>
+      <c r="C7" s="17">
+        <v>0</v>
+      </c>
+      <c r="D7" s="17">
+        <v>0</v>
+      </c>
+      <c r="E7" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" s="3" customFormat="1" spans="1:5">
+      <c r="A8" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="3">
+        <v>0</v>
+      </c>
+      <c r="C8" s="17">
+        <v>0</v>
+      </c>
+      <c r="D8" s="17">
+        <v>0</v>
+      </c>
+      <c r="E8" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" s="3" customFormat="1" spans="1:5">
+      <c r="A9" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="3">
+        <v>0</v>
+      </c>
+      <c r="C9" s="17">
+        <v>0</v>
+      </c>
+      <c r="D9" s="17">
+        <v>0</v>
+      </c>
+      <c r="E9" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" s="4" customFormat="1" ht="14.25" spans="1:5">
+      <c r="A10" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="19"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+    </row>
+    <row r="11" s="28" customFormat="1" spans="1:5">
+      <c r="A11" s="30" t="s">
+        <v>172</v>
+      </c>
+      <c r="C11" s="31" t="s">
+        <v>173</v>
+      </c>
+      <c r="D11"/>
+      <c r="E11"/>
+    </row>
+    <row r="12" s="28" customFormat="1" spans="1:5">
+      <c r="A12" s="30" t="s">
+        <v>174</v>
+      </c>
+      <c r="C12" s="31" t="s">
+        <v>173</v>
+      </c>
+      <c r="D12"/>
+      <c r="E12"/>
+    </row>
+    <row r="13" s="28" customFormat="1" spans="1:5">
+      <c r="A13" s="30" t="s">
+        <v>175</v>
+      </c>
+      <c r="C13" s="31" t="s">
+        <v>173</v>
+      </c>
+      <c r="D13"/>
+      <c r="E13"/>
+    </row>
+    <row r="14" s="28" customFormat="1" spans="1:5">
+      <c r="A14" s="30" t="s">
+        <v>176</v>
+      </c>
+      <c r="C14" s="31" t="s">
+        <v>173</v>
+      </c>
+      <c r="D14"/>
+      <c r="E14"/>
+    </row>
+    <row r="15" s="28" customFormat="1" spans="1:5">
+      <c r="A15" s="30" t="s">
+        <v>177</v>
+      </c>
+      <c r="C15" s="31" t="s">
+        <v>173</v>
+      </c>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+    </row>
+    <row r="16" s="28" customFormat="1" spans="1:5">
+      <c r="A16" s="30" t="s">
+        <v>178</v>
+      </c>
+      <c r="C16" s="31" t="s">
+        <v>173</v>
+      </c>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="32" t="s">
+        <v>179</v>
+      </c>
+      <c r="B17" s="32"/>
+      <c r="C17" s="32" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="32" t="s">
+        <v>181</v>
+      </c>
+      <c r="B18" s="32"/>
+      <c r="C18" s="32" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="32" t="s">
+        <v>183</v>
+      </c>
+      <c r="B19" s="32"/>
+      <c r="C19" s="32" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="32" t="s">
+        <v>185</v>
+      </c>
+      <c r="B20" s="32"/>
+      <c r="C20" s="32" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="32" t="s">
+        <v>187</v>
+      </c>
+      <c r="B21" s="32"/>
+      <c r="C21" s="32" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="32" t="s">
+        <v>189</v>
+      </c>
+      <c r="B22" s="32"/>
+      <c r="C22" s="32" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="32" t="s">
+        <v>191</v>
+      </c>
+      <c r="B23" s="32"/>
+      <c r="C23" s="32" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="32" t="s">
+        <v>193</v>
+      </c>
+      <c r="B24" s="32"/>
+      <c r="C24" s="32" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="32" t="s">
+        <v>195</v>
+      </c>
+      <c r="B25" s="32"/>
+      <c r="C25" s="32" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="32" t="s">
+        <v>197</v>
+      </c>
+      <c r="B26" s="32"/>
+      <c r="C26" s="32" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="32" t="s">
+        <v>199</v>
+      </c>
+      <c r="B27" s="32"/>
+      <c r="C27" s="32" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="32" t="s">
+        <v>201</v>
+      </c>
+      <c r="B28" s="32"/>
+      <c r="C28" s="32" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="32" t="s">
+        <v>203</v>
+      </c>
+      <c r="B29" s="32"/>
+      <c r="C29" s="32" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" s="32" t="s">
+        <v>205</v>
+      </c>
+      <c r="B30" s="32"/>
+      <c r="C30" s="32" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" s="32" t="s">
+        <v>207</v>
+      </c>
+      <c r="B31" s="32"/>
+      <c r="C31" s="32" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" s="32" t="s">
+        <v>209</v>
+      </c>
+      <c r="B32" s="32"/>
+      <c r="C32" s="32" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="32" t="s">
+        <v>211</v>
+      </c>
+      <c r="B33" s="32"/>
+      <c r="C33" s="32" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="32" t="s">
+        <v>213</v>
+      </c>
+      <c r="B34" s="32"/>
+      <c r="C34" s="32" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="32" t="s">
+        <v>215</v>
+      </c>
+      <c r="B35" s="32"/>
+      <c r="C35" s="32" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="32" t="s">
+        <v>217</v>
+      </c>
+      <c r="B36" s="32"/>
+      <c r="C36" s="32" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" s="32" t="s">
+        <v>219</v>
+      </c>
+      <c r="B37" s="32"/>
+      <c r="C37" s="32" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" s="32" t="s">
+        <v>221</v>
+      </c>
+      <c r="B38" s="32"/>
+      <c r="C38" s="32" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" s="32" t="s">
+        <v>223</v>
+      </c>
+      <c r="B39" s="32"/>
+      <c r="C39" s="32" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" s="32" t="s">
+        <v>225</v>
+      </c>
+      <c r="B40" s="32"/>
+      <c r="C40" s="32" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" s="32" t="s">
+        <v>227</v>
+      </c>
+      <c r="B41" s="32"/>
+      <c r="C41" s="32" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" s="32" t="s">
+        <v>229</v>
+      </c>
+      <c r="B42" s="32"/>
+      <c r="C42" s="32" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" s="32" t="s">
+        <v>231</v>
+      </c>
+      <c r="B43" s="32"/>
+      <c r="C43" s="32" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" s="32" t="s">
+        <v>233</v>
+      </c>
+      <c r="B44" s="32"/>
+      <c r="C44" s="32" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" s="32" t="s">
+        <v>235</v>
+      </c>
+      <c r="B45" s="32"/>
+      <c r="C45" s="32" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" s="32" t="s">
+        <v>237</v>
+      </c>
+      <c r="B46" s="32"/>
+      <c r="C46" s="32" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" s="32" t="s">
+        <v>239</v>
+      </c>
+      <c r="B47" s="32"/>
+      <c r="C47" s="32" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" s="32" t="s">
+        <v>241</v>
+      </c>
+      <c r="B48" s="32"/>
+      <c r="C48" s="32" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" s="32" t="s">
+        <v>243</v>
+      </c>
+      <c r="B49" s="32"/>
+      <c r="C49" s="32" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" s="32" t="s">
+        <v>245</v>
+      </c>
+      <c r="B50" s="32"/>
+      <c r="C50" s="32" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" s="32" t="s">
+        <v>247</v>
+      </c>
+      <c r="B51" s="32"/>
+      <c r="C51" s="32" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" s="32" t="s">
+        <v>249</v>
+      </c>
+      <c r="B52" s="32"/>
+      <c r="C52" s="32" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53" s="32" t="s">
+        <v>251</v>
+      </c>
+      <c r="B53" s="32"/>
+      <c r="C53" s="32" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54" s="32" t="s">
+        <v>252</v>
+      </c>
+      <c r="B54" s="32"/>
+      <c r="C54" s="32" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="A55" s="32" t="s">
+        <v>253</v>
+      </c>
+      <c r="B55" s="32"/>
+      <c r="C55" s="32" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56" s="32" t="s">
+        <v>254</v>
+      </c>
+      <c r="B56" s="32"/>
+      <c r="C56" s="32" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57" s="32" t="s">
+        <v>255</v>
+      </c>
+      <c r="B57" s="32"/>
+      <c r="C57" s="32" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="A58" s="32" t="s">
+        <v>256</v>
+      </c>
+      <c r="B58" s="32"/>
+      <c r="C58" s="32" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
+      <c r="A59" s="32" t="s">
+        <v>257</v>
+      </c>
+      <c r="B59" s="32"/>
+      <c r="C59" s="32" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
+      <c r="A60" s="32" t="s">
+        <v>258</v>
+      </c>
+      <c r="B60" s="32"/>
+      <c r="C60" s="32" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
+      <c r="A61" s="32" t="s">
+        <v>259</v>
+      </c>
+      <c r="B61" s="32"/>
+      <c r="C61" s="32" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
+      <c r="A62" s="32" t="s">
+        <v>260</v>
+      </c>
+      <c r="B62" s="32"/>
+      <c r="C62" s="32" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3">
+      <c r="A63" s="32" t="s">
+        <v>261</v>
+      </c>
+      <c r="B63" s="32"/>
+      <c r="C63" s="32" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
+      <c r="A64" s="32" t="s">
+        <v>262</v>
+      </c>
+      <c r="B64" s="32"/>
+      <c r="C64" s="32" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
+      <c r="A65" s="32" t="s">
+        <v>263</v>
+      </c>
+      <c r="B65" s="32"/>
+      <c r="C65" s="32" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
+      <c r="A66" s="32" t="s">
+        <v>264</v>
+      </c>
+      <c r="B66" s="32"/>
+      <c r="C66" s="32" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
+      <c r="A67" s="32" t="s">
+        <v>265</v>
+      </c>
+      <c r="B67" s="32"/>
+      <c r="C67" s="32" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="A68" s="32" t="s">
+        <v>266</v>
+      </c>
+      <c r="B68" s="32"/>
+      <c r="C68" s="32" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
+      <c r="A69" s="32" t="s">
+        <v>267</v>
+      </c>
+      <c r="B69" s="32"/>
+      <c r="C69" s="32" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
+      <c r="A70" s="32" t="s">
+        <v>268</v>
+      </c>
+      <c r="B70" s="32"/>
+      <c r="C70" s="32" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3">
+      <c r="A71" s="32" t="s">
+        <v>269</v>
+      </c>
+      <c r="B71" s="32"/>
+      <c r="C71" s="32" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3">
+      <c r="A72" s="32" t="s">
+        <v>270</v>
+      </c>
+      <c r="B72" s="32"/>
+      <c r="C72" s="32" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3">
+      <c r="A73" s="32" t="s">
+        <v>271</v>
+      </c>
+      <c r="B73" s="32"/>
+      <c r="C73" s="32" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3">
+      <c r="A74" s="32" t="s">
+        <v>272</v>
+      </c>
+      <c r="B74" s="32"/>
+      <c r="C74" s="32" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3">
+      <c r="A75" s="32" t="s">
+        <v>273</v>
+      </c>
+      <c r="B75" s="32"/>
+      <c r="C75" s="32" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3">
+      <c r="A76" s="32" t="s">
+        <v>274</v>
+      </c>
+      <c r="B76" s="32"/>
+      <c r="C76" s="32" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3">
+      <c r="A77" s="32" t="s">
+        <v>275</v>
+      </c>
+      <c r="B77" s="32"/>
+      <c r="C77" s="32" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3">
+      <c r="A78" s="32" t="s">
+        <v>276</v>
+      </c>
+      <c r="B78" s="32"/>
+      <c r="C78" s="32" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3">
+      <c r="A79" s="32" t="s">
+        <v>277</v>
+      </c>
+      <c r="B79" s="32"/>
+      <c r="C79" s="32" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3">
+      <c r="A80" s="32" t="s">
+        <v>278</v>
+      </c>
+      <c r="B80" s="32"/>
+      <c r="C80" s="32" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3">
+      <c r="A81" s="32" t="s">
+        <v>279</v>
+      </c>
+      <c r="B81" s="32"/>
+      <c r="C81" s="32" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3">
+      <c r="A82" s="32" t="s">
+        <v>280</v>
+      </c>
+      <c r="B82" s="32"/>
+      <c r="C82" s="32" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3">
+      <c r="A83" s="32" t="s">
+        <v>281</v>
+      </c>
+      <c r="B83" s="32"/>
+      <c r="C83" s="32" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3">
+      <c r="A84" s="32" t="s">
+        <v>282</v>
+      </c>
+      <c r="B84" s="32"/>
+      <c r="C84" s="32" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3">
+      <c r="A85" s="32" t="s">
+        <v>283</v>
+      </c>
+      <c r="B85" s="32"/>
+      <c r="C85" s="32" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3">
+      <c r="A86" s="32" t="s">
+        <v>284</v>
+      </c>
+      <c r="B86" s="32"/>
+      <c r="C86" s="32" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3">
+      <c r="A87" s="32" t="s">
+        <v>285</v>
+      </c>
+      <c r="B87" s="32"/>
+      <c r="C87" s="32" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3">
+      <c r="A88" s="32" t="s">
+        <v>286</v>
+      </c>
+      <c r="B88" s="32"/>
+      <c r="C88" s="32" t="s">
+        <v>250</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="2">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A6:A9"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D6:D9 E6:E9 B6:C9">
+      <formula1>"TRUE,FALSE"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter alignWithMargins="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:E30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="10" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection/>
+      <selection pane="bottomLeft" activeCell="A31" sqref="$A31:$XFD36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="4"/>
+  <cols>
+    <col min="1" max="1" width="31.8" style="5" customWidth="1"/>
+    <col min="2" max="2" width="33.3333333333333" style="6" customWidth="1"/>
+    <col min="3" max="3" width="87.4" style="7" customWidth="1"/>
+    <col min="4" max="16384" width="9" style="8"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" spans="1:5">
+      <c r="A1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" s="2" customFormat="1" spans="1:5">
+      <c r="A2" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" s="2" customFormat="1" spans="1:5">
+      <c r="A3" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="2">
+        <v>0</v>
+      </c>
+      <c r="C3" s="15">
+        <v>0</v>
+      </c>
+      <c r="D3" s="15">
+        <v>0</v>
+      </c>
+      <c r="E3" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" s="2" customFormat="1" spans="1:5">
+      <c r="A4" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0</v>
+      </c>
+      <c r="C4" s="15">
+        <v>0</v>
+      </c>
+      <c r="D4" s="15">
+        <v>0</v>
+      </c>
+      <c r="E4" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" s="2" customFormat="1" spans="1:5">
+      <c r="A5" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="2">
+        <v>0</v>
+      </c>
+      <c r="C5" s="15">
+        <v>0</v>
+      </c>
+      <c r="D5" s="15">
+        <v>0</v>
+      </c>
+      <c r="E5" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" s="2" customFormat="1" spans="1:5">
+      <c r="A6" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="2">
+        <v>0</v>
+      </c>
+      <c r="C6" s="15">
+        <v>0</v>
+      </c>
+      <c r="D6" s="15">
+        <v>0</v>
+      </c>
+      <c r="E6" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" s="3" customFormat="1" spans="1:5">
+      <c r="A7" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="3">
+        <v>0</v>
+      </c>
+      <c r="C7" s="17">
+        <v>0</v>
+      </c>
+      <c r="D7" s="17">
+        <v>0</v>
+      </c>
+      <c r="E7" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" s="3" customFormat="1" spans="1:5">
+      <c r="A8" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="3">
+        <v>0</v>
+      </c>
+      <c r="C8" s="17">
+        <v>0</v>
+      </c>
+      <c r="D8" s="17">
+        <v>0</v>
+      </c>
+      <c r="E8" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" s="3" customFormat="1" spans="1:5">
+      <c r="A9" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="3">
+        <v>0</v>
+      </c>
+      <c r="C9" s="17">
+        <v>0</v>
+      </c>
+      <c r="D9" s="17">
+        <v>0</v>
+      </c>
+      <c r="E9" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" s="4" customFormat="1" ht="14.25" spans="1:5">
+      <c r="A10" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="19"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+    </row>
+    <row r="11" s="22" customFormat="1" spans="1:5">
+      <c r="A11" s="21" t="s">
+        <v>287</v>
+      </c>
+      <c r="C11" s="23" t="s">
+        <v>288</v>
+      </c>
+      <c r="D11" s="24"/>
+      <c r="E11" s="24"/>
+    </row>
+    <row r="12" s="25" customFormat="1" spans="1:5">
+      <c r="A12" s="29" t="s">
+        <v>289</v>
+      </c>
+      <c r="C12" s="26" t="s">
+        <v>290</v>
+      </c>
+      <c r="D12" s="27"/>
+      <c r="E12" s="27"/>
+    </row>
+    <row r="13" s="22" customFormat="1" spans="1:5">
+      <c r="A13" s="21" t="s">
+        <v>291</v>
+      </c>
+      <c r="C13" s="23" t="s">
+        <v>292</v>
+      </c>
+      <c r="D13" s="27"/>
+      <c r="E13" s="27"/>
+    </row>
+    <row r="14" s="25" customFormat="1" spans="1:5">
+      <c r="A14" s="29" t="s">
+        <v>293</v>
+      </c>
+      <c r="C14" s="26" t="s">
+        <v>294</v>
+      </c>
+      <c r="D14" s="27"/>
+      <c r="E14" s="27"/>
+    </row>
+    <row r="15" s="25" customFormat="1" spans="1:5">
+      <c r="A15" s="29" t="s">
+        <v>295</v>
+      </c>
+      <c r="C15" s="26" t="s">
+        <v>296</v>
+      </c>
+      <c r="D15" s="27"/>
+      <c r="E15" s="27"/>
+    </row>
+    <row r="16" s="25" customFormat="1" spans="1:5">
+      <c r="A16" s="29" t="s">
+        <v>297</v>
+      </c>
+      <c r="C16" s="26" t="s">
+        <v>298</v>
+      </c>
+      <c r="D16" s="27"/>
+      <c r="E16" s="27"/>
+    </row>
+    <row r="17" s="25" customFormat="1" spans="1:5">
+      <c r="A17" s="29" t="s">
+        <v>299</v>
+      </c>
+      <c r="C17" s="26" t="s">
+        <v>300</v>
+      </c>
+      <c r="D17" s="24"/>
+      <c r="E17" s="24"/>
+    </row>
+    <row r="18" s="25" customFormat="1" spans="1:5">
+      <c r="A18" s="29" t="s">
+        <v>301</v>
+      </c>
+      <c r="C18" s="26" t="s">
+        <v>302</v>
+      </c>
+      <c r="D18" s="27"/>
+      <c r="E18" s="27"/>
+    </row>
+    <row r="19" s="25" customFormat="1" spans="1:5">
+      <c r="A19" s="29" t="s">
+        <v>303</v>
+      </c>
+      <c r="C19" s="26" t="s">
+        <v>304</v>
+      </c>
+      <c r="D19" s="27"/>
+      <c r="E19" s="27"/>
+    </row>
+    <row r="20" s="25" customFormat="1" spans="1:5">
+      <c r="A20" s="29" t="s">
+        <v>305</v>
+      </c>
+      <c r="C20" s="26" t="s">
+        <v>306</v>
+      </c>
+      <c r="D20" s="27"/>
+      <c r="E20" s="27"/>
+    </row>
+    <row r="21" s="28" customFormat="1" spans="1:5">
+      <c r="A21" s="30" t="s">
+        <v>307</v>
+      </c>
+      <c r="C21" s="31" t="s">
+        <v>308</v>
+      </c>
+      <c r="D21"/>
+      <c r="E21"/>
+    </row>
+    <row r="22" s="28" customFormat="1" spans="1:5">
+      <c r="A22" s="30" t="s">
+        <v>309</v>
+      </c>
+      <c r="C22" s="31" t="s">
+        <v>310</v>
+      </c>
+      <c r="D22"/>
+      <c r="E22"/>
+    </row>
+    <row r="23" s="28" customFormat="1" spans="1:5">
+      <c r="A23" s="30" t="s">
+        <v>311</v>
+      </c>
+      <c r="C23" s="31" t="s">
+        <v>312</v>
+      </c>
+      <c r="D23"/>
+      <c r="E23"/>
+    </row>
+    <row r="24" s="28" customFormat="1" spans="1:5">
+      <c r="A24" s="30" t="s">
+        <v>313</v>
+      </c>
+      <c r="C24" s="31" t="s">
+        <v>314</v>
+      </c>
+      <c r="D24"/>
+      <c r="E24"/>
+    </row>
+    <row r="25" s="28" customFormat="1" spans="1:5">
+      <c r="A25" s="30" t="s">
+        <v>315</v>
+      </c>
+      <c r="C25" s="31" t="s">
+        <v>316</v>
+      </c>
+      <c r="D25"/>
+      <c r="E25"/>
+    </row>
+    <row r="26" s="28" customFormat="1" spans="1:5">
+      <c r="A26" s="30" t="s">
+        <v>317</v>
+      </c>
+      <c r="C26" s="31" t="s">
+        <v>318</v>
+      </c>
+      <c r="D26"/>
+      <c r="E26"/>
+    </row>
+    <row r="27" s="28" customFormat="1" spans="1:5">
+      <c r="A27" s="30" t="s">
+        <v>319</v>
+      </c>
+      <c r="C27" s="31" t="s">
+        <v>320</v>
+      </c>
+      <c r="D27"/>
+      <c r="E27"/>
+    </row>
+    <row r="28" s="28" customFormat="1" spans="1:5">
+      <c r="A28" s="30" t="s">
+        <v>321</v>
+      </c>
+      <c r="C28" s="31" t="s">
+        <v>322</v>
+      </c>
+      <c r="D28"/>
+      <c r="E28"/>
+    </row>
+    <row r="29" s="28" customFormat="1" spans="1:5">
+      <c r="A29" s="30" t="s">
+        <v>323</v>
+      </c>
+      <c r="C29" s="31" t="s">
+        <v>324</v>
+      </c>
+      <c r="D29"/>
+      <c r="E29"/>
+    </row>
+    <row r="30" s="28" customFormat="1" spans="1:5">
+      <c r="A30" s="30" t="s">
+        <v>325</v>
+      </c>
+      <c r="C30" s="31" t="s">
+        <v>326</v>
+      </c>
+      <c r="D30"/>
+      <c r="E30"/>
+    </row>
+  </sheetData>
+  <dataValidations count="2">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A6:A9"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D6:D9 E6:E9 B6:C9">
+      <formula1>"TRUE,FALSE"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter alignWithMargins="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:E10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="10" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection/>
+      <selection pane="bottomLeft" activeCell="A122" sqref="$A11:$XFD122"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="4"/>
+  <cols>
+    <col min="1" max="1" width="31.8" style="5" customWidth="1"/>
+    <col min="2" max="2" width="33.3333333333333" style="6" customWidth="1"/>
+    <col min="3" max="3" width="87.4" style="7" customWidth="1"/>
+    <col min="4" max="16384" width="9" style="8"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" spans="1:5">
+      <c r="A1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" s="2" customFormat="1" spans="1:5">
+      <c r="A2" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" s="2" customFormat="1" spans="1:5">
+      <c r="A3" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="2">
+        <v>0</v>
+      </c>
+      <c r="C3" s="15">
+        <v>0</v>
+      </c>
+      <c r="D3" s="15">
+        <v>0</v>
+      </c>
+      <c r="E3" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" s="2" customFormat="1" spans="1:5">
+      <c r="A4" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0</v>
+      </c>
+      <c r="C4" s="15">
+        <v>0</v>
+      </c>
+      <c r="D4" s="15">
+        <v>0</v>
+      </c>
+      <c r="E4" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" s="2" customFormat="1" spans="1:5">
+      <c r="A5" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="2">
+        <v>0</v>
+      </c>
+      <c r="C5" s="15">
+        <v>0</v>
+      </c>
+      <c r="D5" s="15">
+        <v>0</v>
+      </c>
+      <c r="E5" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" s="2" customFormat="1" spans="1:5">
+      <c r="A6" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="2">
+        <v>0</v>
+      </c>
+      <c r="C6" s="15">
+        <v>0</v>
+      </c>
+      <c r="D6" s="15">
+        <v>0</v>
+      </c>
+      <c r="E6" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" s="3" customFormat="1" spans="1:5">
+      <c r="A7" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="3">
+        <v>0</v>
+      </c>
+      <c r="C7" s="17">
+        <v>0</v>
+      </c>
+      <c r="D7" s="17">
+        <v>0</v>
+      </c>
+      <c r="E7" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" s="3" customFormat="1" spans="1:5">
+      <c r="A8" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="3">
+        <v>0</v>
+      </c>
+      <c r="C8" s="17">
+        <v>0</v>
+      </c>
+      <c r="D8" s="17">
+        <v>0</v>
+      </c>
+      <c r="E8" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" s="3" customFormat="1" spans="1:5">
+      <c r="A9" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="3">
+        <v>0</v>
+      </c>
+      <c r="C9" s="17">
+        <v>0</v>
+      </c>
+      <c r="D9" s="17">
+        <v>0</v>
+      </c>
+      <c r="E9" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" s="4" customFormat="1" ht="14.25" spans="1:5">
+      <c r="A10" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="19"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+    </row>
+  </sheetData>
+  <dataValidations count="2">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A6:A9"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D6:D9 E6:E9 B6:C9">
+      <formula1>"TRUE,FALSE"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter alignWithMargins="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:E48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="10" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
       <selection/>
       <selection pane="bottomLeft" activeCell="C19" sqref="C19"/>

</xml_diff>